<commit_message>
merge #2, ProjectObject branch successfully integrated
</commit_message>
<xml_diff>
--- a/PMConverter/src/test2.xlsx
+++ b/PMConverter/src/test2.xlsx
@@ -669,34 +669,67 @@
     <t>Assigned To</t>
   </si>
   <si>
+    <t>plasterer</t>
+  </si>
+  <si>
+    <t>RENEWABLE</t>
+  </si>
+  <si>
+    <t>4 #4</t>
+  </si>
+  <si>
+    <t>32[3 #4];</t>
+  </si>
+  <si>
+    <t>joiner</t>
+  </si>
+  <si>
+    <t>5 #5</t>
+  </si>
+  <si>
+    <t>40[5 #5];</t>
+  </si>
+  <si>
+    <t>27;45;55;</t>
+  </si>
+  <si>
+    <t>30;52;53;</t>
+  </si>
+  <si>
+    <t>29;51;61;54;</t>
+  </si>
+  <si>
+    <t>roofer</t>
+  </si>
+  <si>
+    <t>49[4 #4];</t>
+  </si>
+  <si>
     <t>painter</t>
   </si>
   <si>
-    <t>Renewable</t>
-  </si>
-  <si>
     <t>6 #6</t>
   </si>
   <si>
     <t>39[4 #6];</t>
   </si>
   <si>
-    <t>joiner</t>
-  </si>
-  <si>
-    <t>5 #5</t>
-  </si>
-  <si>
-    <t>40[5 #5];</t>
-  </si>
-  <si>
-    <t>roofer</t>
-  </si>
-  <si>
-    <t>4 #4</t>
-  </si>
-  <si>
-    <t>49[4 #4];</t>
+    <t>3 #3</t>
+  </si>
+  <si>
+    <t>34[2 #3];56;</t>
+  </si>
+  <si>
+    <t>carpenter</t>
+  </si>
+  <si>
+    <t>26[3 #3];</t>
+  </si>
+  <si>
+    <t>8 #8</t>
+  </si>
+  <si>
+    <t>6[4 #8];17;69;18[3 #8];21[3 #8];23[5 #8];19[4 #8];20[4 #8];22[3 #8];24[4 #8];25[2 #8];28[5 #8];</t>
   </si>
   <si>
     <t>2 #2</t>
@@ -705,42 +738,9 @@
     <t>59;60;</t>
   </si>
   <si>
-    <t>plasterer</t>
-  </si>
-  <si>
-    <t>32[3 #4];</t>
-  </si>
-  <si>
-    <t>27;45;55;</t>
-  </si>
-  <si>
-    <t>3 #3</t>
-  </si>
-  <si>
-    <t>34[2 #3];56;</t>
-  </si>
-  <si>
-    <t>30;52;53;</t>
-  </si>
-  <si>
-    <t>8 #8</t>
-  </si>
-  <si>
-    <t>6[4 #8];17;69;18[3 #8];21[3 #8];23[5 #8];19[4 #8];20[4 #8];22[3 #8];24[4 #8];25[2 #8];28[5 #8];</t>
-  </si>
-  <si>
-    <t>carpenter</t>
-  </si>
-  <si>
-    <t>26[3 #3];</t>
-  </si>
-  <si>
     <t>35;57;58;</t>
   </si>
   <si>
-    <t>29;51;61;54;</t>
-  </si>
-  <si>
     <t>Activity Duration Distribution Profiles</t>
   </si>
   <si>
@@ -756,16 +756,16 @@
     <t>Pessimistic</t>
   </si>
   <si>
-    <t>manual - absolute</t>
-  </si>
-  <si>
-    <t>standard - symmetric</t>
-  </si>
-  <si>
-    <t>standard - no risk</t>
-  </si>
-  <si>
-    <t>standard - skewed left</t>
+    <t>MANUAL - ABSOLUTE</t>
+  </si>
+  <si>
+    <t>STANDARD - SYMMETRIC</t>
+  </si>
+  <si>
+    <t>STANDARD - NO_RISK</t>
+  </si>
+  <si>
+    <t>STANDARD - SKEWED_LEFT</t>
   </si>
 </sst>
 </file>
@@ -3783,6 +3783,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3829,7 +3830,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>217</v>
@@ -3844,13 +3845,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="13">
-        <v>35</v>
+        <v>41.38</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>220</v>
       </c>
       <c r="H3" s="5">
-        <v>16800</v>
+        <v>14896.8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3881,262 +3882,262 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>224</v>
+        <v>116</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
       </c>
       <c r="F5" s="13">
-        <v>36</v>
+        <v>40.65</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H5" s="5">
-        <v>11520</v>
+        <v>9756</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="E6" s="13">
         <v>0</v>
       </c>
       <c r="F6" s="13">
-        <v>43.2</v>
+        <v>36</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H6" s="5">
-        <v>13824</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>229</v>
+        <v>123</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
       <c r="F7" s="13">
-        <v>41.38</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H7" s="5">
-        <v>14896.8</v>
+        <v>24320</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>116</v>
+        <v>227</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
       </c>
       <c r="F8" s="13">
-        <v>40.65</v>
+        <v>36</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H8" s="5">
-        <v>9756</v>
+        <v>11520</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>166</v>
+        <v>229</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E9" s="13">
         <v>0</v>
       </c>
       <c r="F9" s="13">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>16800</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>113</v>
+        <v>166</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E10" s="13">
         <v>0</v>
       </c>
       <c r="F10" s="13">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H10" s="5">
-        <v>8640</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>234</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>38.56</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>236</v>
-      </c>
       <c r="H11" s="5">
-        <v>173057.28</v>
+        <v>9120</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>237</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E12" s="13">
         <v>0</v>
       </c>
       <c r="F12" s="13">
-        <v>38</v>
+        <v>38.56</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H12" s="5">
-        <v>9120</v>
+        <v>173057.28</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c r="E13" s="13">
         <v>0</v>
       </c>
       <c r="F13" s="13">
-        <v>41.56</v>
+        <v>43.2</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>239</v>
       </c>
       <c r="H13" s="5">
-        <v>19948.8</v>
+        <v>13824</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="E14" s="13">
         <v>0</v>
       </c>
       <c r="F14" s="13">
-        <v>32</v>
+        <v>41.56</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>240</v>
       </c>
       <c r="H14" s="5">
-        <v>24320</v>
+        <v>19948.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished reading tracking periods
</commit_message>
<xml_diff>
--- a/PMConverter/src/test2.xlsx
+++ b/PMConverter/src/test2.xlsx
@@ -669,76 +669,76 @@
     <t>Assigned To</t>
   </si>
   <si>
+    <t>joiner</t>
+  </si>
+  <si>
+    <t>RENEWABLE</t>
+  </si>
+  <si>
+    <t>5 #5</t>
+  </si>
+  <si>
+    <t>40[5 #5];</t>
+  </si>
+  <si>
+    <t>roofer</t>
+  </si>
+  <si>
+    <t>4 #4</t>
+  </si>
+  <si>
+    <t>49[4 #4];</t>
+  </si>
+  <si>
+    <t>30;52;53;</t>
+  </si>
+  <si>
+    <t>8 #8</t>
+  </si>
+  <si>
+    <t>6[4 #8];17;18[3 #8];19[4 #8];20[4 #8];21[3 #8];22[3 #8];23[5 #8];24[4 #8];25[2 #8];28[5 #8];69;</t>
+  </si>
+  <si>
+    <t>27;45;55;</t>
+  </si>
+  <si>
+    <t>29;51;54;61;</t>
+  </si>
+  <si>
+    <t>2 #2</t>
+  </si>
+  <si>
+    <t>59;60;</t>
+  </si>
+  <si>
+    <t>3 #3</t>
+  </si>
+  <si>
+    <t>34[2 #3];56;</t>
+  </si>
+  <si>
+    <t>carpenter</t>
+  </si>
+  <si>
+    <t>26[3 #3];</t>
+  </si>
+  <si>
+    <t>painter</t>
+  </si>
+  <si>
+    <t>6 #6</t>
+  </si>
+  <si>
+    <t>39[4 #6];</t>
+  </si>
+  <si>
+    <t>35;57;58;</t>
+  </si>
+  <si>
     <t>plasterer</t>
   </si>
   <si>
-    <t>RENEWABLE</t>
-  </si>
-  <si>
-    <t>4 #4</t>
-  </si>
-  <si>
     <t>32[3 #4];</t>
-  </si>
-  <si>
-    <t>35;57;58;</t>
-  </si>
-  <si>
-    <t>roofer</t>
-  </si>
-  <si>
-    <t>49[4 #4];</t>
-  </si>
-  <si>
-    <t>joiner</t>
-  </si>
-  <si>
-    <t>5 #5</t>
-  </si>
-  <si>
-    <t>40[5 #5];</t>
-  </si>
-  <si>
-    <t>carpenter</t>
-  </si>
-  <si>
-    <t>3 #3</t>
-  </si>
-  <si>
-    <t>26[3 #3];</t>
-  </si>
-  <si>
-    <t>8 #8</t>
-  </si>
-  <si>
-    <t>6[4 #8];17;18[3 #8];19[4 #8];20[4 #8];21[3 #8];22[3 #8];23[5 #8];24[4 #8];25[2 #8];28[5 #8];69;</t>
-  </si>
-  <si>
-    <t>2 #2</t>
-  </si>
-  <si>
-    <t>59;60;</t>
-  </si>
-  <si>
-    <t>29;51;54;61;</t>
-  </si>
-  <si>
-    <t>27;45;55;</t>
-  </si>
-  <si>
-    <t>painter</t>
-  </si>
-  <si>
-    <t>6 #6</t>
-  </si>
-  <si>
-    <t>39[4 #6];</t>
-  </si>
-  <si>
-    <t>34[2 #3];56;</t>
-  </si>
-  <si>
-    <t>30;52;53;</t>
   </si>
   <si>
     <t>Activity Duration Distribution Profiles</t>
@@ -3830,7 +3830,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>217</v>
@@ -3845,53 +3845,53 @@
         <v>0</v>
       </c>
       <c r="F3" s="13">
-        <v>41.38</v>
+        <v>42</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>220</v>
       </c>
       <c r="H3" s="5">
-        <v>14896.8</v>
+        <v>8400</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E4" s="13">
         <v>0</v>
       </c>
       <c r="F4" s="13">
-        <v>41.56</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H4" s="5">
-        <v>19948.8</v>
+        <v>11520</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>222</v>
+        <v>100</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
@@ -3900,18 +3900,18 @@
         <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H5" s="5">
-        <v>11520</v>
+        <v>8640</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>224</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>218</v>
@@ -3923,65 +3923,65 @@
         <v>0</v>
       </c>
       <c r="F6" s="13">
-        <v>42</v>
+        <v>38.56</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>226</v>
       </c>
       <c r="H6" s="5">
-        <v>8400</v>
+        <v>173057.28</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>227</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E7" s="13">
         <v>0</v>
       </c>
       <c r="F7" s="13">
-        <v>38</v>
+        <v>40.65</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H7" s="5">
-        <v>9120</v>
+        <v>9756</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
       </c>
       <c r="F8" s="13">
-        <v>38.56</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H8" s="5">
-        <v>173057.28</v>
+        <v>24320</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3995,7 +3995,7 @@
         <v>218</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E9" s="13">
         <v>0</v>
@@ -4004,7 +4004,7 @@
         <v>43.2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="H9" s="5">
         <v>13824</v>
@@ -4012,54 +4012,54 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>97</v>
+        <v>174</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E10" s="13">
         <v>0</v>
       </c>
       <c r="F10" s="13">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="H10" s="5">
-        <v>24320</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>89</v>
+        <v>233</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="E11" s="13">
         <v>0</v>
       </c>
       <c r="F11" s="13">
-        <v>40.65</v>
+        <v>38</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H11" s="5">
-        <v>9756</v>
+        <v>9120</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -4067,13 +4067,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E12" s="13">
         <v>0</v>
@@ -4082,7 +4082,7 @@
         <v>35</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H12" s="5">
         <v>16800</v>
@@ -4090,54 +4090,54 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>174</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E13" s="13">
         <v>0</v>
       </c>
       <c r="F13" s="13">
-        <v>0</v>
+        <v>41.56</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H13" s="5">
-        <v>0</v>
+        <v>19948.8</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>218</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E14" s="13">
         <v>0</v>
       </c>
       <c r="F14" s="13">
-        <v>36</v>
+        <v>41.38</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>240</v>
       </c>
       <c r="H14" s="5">
-        <v>8640</v>
+        <v>14896.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>